<commit_message>
Edit profile page created
</commit_message>
<xml_diff>
--- a/backend/income_details.xlsx
+++ b/backend/income_details.xlsx
@@ -415,24 +415,24 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>rrfcrfr</v>
+        <v>sal</v>
       </c>
       <c r="B2">
-        <v>242</v>
+        <v>12</v>
       </c>
       <c r="C2" t="str">
-        <v>4/24/42242</v>
+        <v>3/23/2025</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>fevfe</v>
+        <v>ww</v>
       </c>
       <c r="B3">
-        <v>24424</v>
+        <v>22</v>
       </c>
       <c r="C3" t="str">
-        <v>2/24/24</v>
+        <v>3/23/2025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>